<commit_message>
Tweaks and Updates from Zach feed back on 1.0.5.1
</commit_message>
<xml_diff>
--- a/orion.web/docs/DetailedExpenseReportTemplate.xlsx
+++ b/orion.web/docs/DetailedExpenseReportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Job</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Grand Total All Expenses</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -466,13 +469,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -587,6 +605,15 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -604,6 +631,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1693,7 +1729,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1899,18 +1935,18 @@
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="27"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" ht="19.5" customHeight="1">
       <c r="A17" t="s" s="33">
         <v>22</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="32"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" ht="16.5" customHeight="1">
       <c r="A18" t="s" s="28">
@@ -1918,35 +1954,37 @@
       </c>
       <c r="B18" s="29"/>
       <c r="C18" t="s" s="30">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s" s="30">
         <v>24</v>
       </c>
-      <c r="D18" t="s" s="30">
+      <c r="E18" t="s" s="30">
         <v>25</v>
       </c>
-      <c r="E18" t="s" s="30">
+      <c r="F18" t="s" s="30">
         <v>26</v>
       </c>
-      <c r="F18" t="s" s="31">
+      <c r="G18" t="s" s="31">
         <v>27</v>
       </c>
-      <c r="G18" s="32"/>
     </row>
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="27"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" ht="14.05" customHeight="1">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43"/>
       <c r="G20" s="27"/>
     </row>
     <row r="21" ht="20.25" customHeight="1">
@@ -1961,19 +1999,19 @@
       <c r="G21" s="27"/>
     </row>
     <row r="22" ht="16.15" customHeight="1">
-      <c r="A22" t="s" s="41">
+      <c r="A22" t="s" s="44">
         <v>29</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="46"/>
       <c r="E22" t="s" s="31">
         <v>12</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="27"/>
     </row>
-    <row r="23" ht="13.55" customHeight="1">
+    <row r="23" ht="14.05" customHeight="1">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -1982,35 +2020,46 @@
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
     </row>
-    <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
+    <row r="24" ht="14.05" customHeight="1">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
     </row>
-    <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" s="44"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
+    <row r="25" ht="18.9" customHeight="1">
+      <c r="A25" t="s" s="22">
+        <v>30</v>
+      </c>
+      <c r="B25" s="47"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
     </row>
     <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" s="44"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
     </row>
+    <row r="27" ht="13.55" customHeight="1">
+      <c r="A27" s="50"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A10:B10"/>
@@ -2020,12 +2069,13 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="88" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>